<commit_message>
Final commit with resultados excel
</commit_message>
<xml_diff>
--- a/Resultados.xlsx
+++ b/Resultados.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wacalvo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wacalvo\IdeaProjects\ProyectoFInal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D636D03-BE59-4BD0-8AF7-E7C198457D66}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D626D1-BBF2-4971-A41D-EB3EC4C6177F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{4CB383B9-BB1C-451D-8F30-A8C7C9238544}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="29">
   <si>
     <t>Tiempo en Espera</t>
   </si>
@@ -79,6 +79,39 @@
   </si>
   <si>
     <t>abiertas</t>
+  </si>
+  <si>
+    <t>Simulacion de Ignacio</t>
+  </si>
+  <si>
+    <t>Relacion Costo/Beneficio</t>
+  </si>
+  <si>
+    <t>El mejor rendimiento se da con 8 cajas.</t>
+  </si>
+  <si>
+    <t>El peor rendimiento se da con 5 cajas.</t>
+  </si>
+  <si>
+    <t>Simulacion de Lolita</t>
+  </si>
+  <si>
+    <t>El mejor rendimiento se da con  8 cajas.</t>
+  </si>
+  <si>
+    <t>El peor rendimiento se da con 3 cajas.</t>
+  </si>
+  <si>
+    <t>Simulacion de Joel</t>
+  </si>
+  <si>
+    <t>El mejor rendimiento se da con 5 cajas.</t>
+  </si>
+  <si>
+    <t>El peor rendimiento se da con 8 cajas.</t>
+  </si>
+  <si>
+    <t>Simulacion de William</t>
   </si>
 </sst>
 </file>
@@ -101,7 +134,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,6 +171,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -166,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -179,6 +218,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C523420E-208C-452D-A877-0CDD6113BE78}">
-  <dimension ref="A1:X36"/>
+  <dimension ref="A1:AB36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K2" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA22" sqref="AA22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -516,9 +559,14 @@
     <col min="13" max="13" width="32" customWidth="1"/>
     <col min="14" max="14" width="27.77734375" customWidth="1"/>
     <col min="15" max="15" width="8.88671875" customWidth="1"/>
+    <col min="20" max="20" width="8.88671875" customWidth="1"/>
+    <col min="26" max="26" width="44.44140625" customWidth="1"/>
+    <col min="27" max="27" width="26.88671875" customWidth="1"/>
+    <col min="28" max="28" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="37.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -540,8 +588,14 @@
       <c r="V1" s="9"/>
       <c r="W1" s="9"/>
       <c r="X1" s="9"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA1" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -585,8 +639,14 @@
       <c r="V2" s="9"/>
       <c r="W2" s="9"/>
       <c r="X2" s="9"/>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA2">
+        <v>2.4700000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>172</v>
       </c>
@@ -632,8 +692,14 @@
       <c r="V3" s="9"/>
       <c r="W3" s="9"/>
       <c r="X3" s="9"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA3">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>190</v>
       </c>
@@ -680,7 +746,7 @@
       <c r="W4" s="9"/>
       <c r="X4" s="9"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>194</v>
       </c>
@@ -724,8 +790,13 @@
       <c r="V5" s="9"/>
       <c r="W5" s="9"/>
       <c r="X5" s="9"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA5" s="11"/>
+      <c r="AB5" s="11"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>184</v>
       </c>
@@ -769,8 +840,14 @@
       <c r="V6" s="9"/>
       <c r="W6" s="9"/>
       <c r="X6" s="9"/>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z6" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA6">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>190</v>
       </c>
@@ -816,8 +893,14 @@
       <c r="V7" s="9"/>
       <c r="W7" s="9"/>
       <c r="X7" s="9"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA7">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>183</v>
       </c>
@@ -864,7 +947,7 @@
       <c r="W8" s="9"/>
       <c r="X8" s="9"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>187</v>
       </c>
@@ -908,8 +991,12 @@
       <c r="V9" s="9"/>
       <c r="W9" s="9"/>
       <c r="X9" s="9"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA9" s="10"/>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>187</v>
       </c>
@@ -953,8 +1040,14 @@
       <c r="V10" s="9"/>
       <c r="W10" s="9"/>
       <c r="X10" s="9"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z10" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA10">
+        <v>4.24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>10</v>
       </c>
@@ -986,8 +1079,20 @@
       <c r="V11" s="9"/>
       <c r="W11" s="9"/>
       <c r="X11" s="9"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA11">
+        <v>4.33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="Z13" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA13" s="10"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>4</v>
       </c>
@@ -1004,8 +1109,14 @@
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z14" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA14">
+        <v>0.468356363</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>0</v>
       </c>
@@ -1042,8 +1153,14 @@
       <c r="N15" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z15" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA15">
+        <v>0.99287469399999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>181</v>
       </c>
@@ -1792,6 +1909,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="AA5:AB5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>

</xml_diff>